<commit_message>
Nothing Updated. Just putting Python script to its new folder - overcut
</commit_message>
<xml_diff>
--- a/data/overcuts.xlsx
+++ b/data/overcuts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Distance</t>
   </si>
@@ -34,7 +34,11 @@
     <t>Tile</t>
   </si>
   <si>
-    <t xml:space="preserve">12in
+    <t xml:space="preserve">12in DW
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10in
 </t>
   </si>
 </sst>
@@ -390,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -421,16 +425,16 @@
         <v>100</v>
       </c>
       <c r="B2" s="2">
-        <v>1346.51</v>
+        <v>1315.51</v>
       </c>
       <c r="C2" s="2">
-        <v>1342.94</v>
+        <v>1312.09</v>
       </c>
       <c r="D2" s="2">
-        <v>3.57</v>
+        <v>3.42</v>
       </c>
       <c r="E2" s="2">
-        <v>3.57</v>
+        <v>3.42</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -441,16 +445,16 @@
         <v>200</v>
       </c>
       <c r="B3" s="2">
-        <v>1347.3</v>
+        <v>1318.29</v>
       </c>
       <c r="C3" s="2">
-        <v>1343.04</v>
+        <v>1314.91</v>
       </c>
       <c r="D3" s="2">
-        <v>4.25</v>
+        <v>3.37</v>
       </c>
       <c r="E3" s="4">
-        <v>4.26</v>
+        <v>3.38</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
@@ -461,19 +465,59 @@
         <v>300</v>
       </c>
       <c r="B4" s="2">
-        <v>1347.34</v>
+        <v>1318.7</v>
       </c>
       <c r="C4" s="2">
-        <v>1343.14</v>
+        <v>1315.15</v>
       </c>
       <c r="D4" s="2">
-        <v>4.19</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4.2</v>
+        <v>3.55</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.55</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>400</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1320.92</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1315.96</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.96</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4.96</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>500</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1324.09</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1316.06</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8.029999999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8.029999999999999</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V2 of Overcuts. This Class works with Excel File V2. It puts all the captured data into the Overcut template file that calculates the overcut depth and shows the tile graph
</commit_message>
<xml_diff>
--- a/data/overcuts.xlsx
+++ b/data/overcuts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Distance</t>
   </si>
@@ -34,11 +34,11 @@
     <t>Tile</t>
   </si>
   <si>
-    <t xml:space="preserve">12in DW
+    <t xml:space="preserve">12in
 </t>
   </si>
   <si>
-    <t xml:space="preserve">10in
+    <t xml:space="preserve">O8in
 </t>
   </si>
 </sst>
@@ -394,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,19 +422,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1315.51</v>
+        <v>1222.55</v>
       </c>
       <c r="C2" s="2">
-        <v>1312.09</v>
+        <v>1219.55</v>
       </c>
       <c r="D2" s="2">
-        <v>3.42</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
-        <v>3.42</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -442,19 +442,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2">
-        <v>1318.29</v>
+        <v>1223.36</v>
       </c>
       <c r="C3" s="2">
-        <v>1314.91</v>
+        <v>1219.79</v>
       </c>
       <c r="D3" s="2">
-        <v>3.37</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3.38</v>
+        <v>3.57</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.57</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
@@ -462,61 +462,201 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="B4" s="2">
-        <v>1318.7</v>
+        <v>1224.34</v>
       </c>
       <c r="C4" s="2">
-        <v>1315.15</v>
+        <v>1219.89</v>
       </c>
       <c r="D4" s="2">
-        <v>3.55</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3.55</v>
+        <v>4.46</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4.45</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2">
-        <v>1320.92</v>
+        <v>1224.84</v>
       </c>
       <c r="C5" s="2">
-        <v>1315.96</v>
+        <v>1219.99</v>
       </c>
       <c r="D5" s="2">
-        <v>4.96</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4.96</v>
+        <v>4.86</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4.85</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
+        <v>400</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1225.53</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1220.09</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5.44</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.44</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
         <v>500</v>
       </c>
-      <c r="B6" s="2">
-        <v>1324.09</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1316.06</v>
-      </c>
-      <c r="D6" s="2">
-        <v>8.029999999999999</v>
-      </c>
-      <c r="E6" s="2">
-        <v>8.029999999999999</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="B7" s="2">
+        <v>1225.09</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1220.19</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.9</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>600</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1225.55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1220.29</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.26</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5.26</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>700</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1225.82</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1220.39</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5.43</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5.43</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>800</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1225.49</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1220.49</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>900</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1225.47</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1220.59</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4.89</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4.88</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1225.5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1220.69</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.81</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4.81</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1225.58</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1220.79</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4.79</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4.79</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>